<commit_message>
update resistor values for VDD sample divider on schematic and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-301-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-301-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EADD52A-9D6C-440A-BFC1-148E3C4CF893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F427C4-9489-40B0-BC3A-032888E061ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="495" windowWidth="24165" windowHeight="14100"/>
+    <workbookView xWindow="30135" yWindow="1155" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="315">
   <si>
     <t>Item</t>
   </si>
@@ -499,9 +499,6 @@
     <t>RC0402FR-071K33L</t>
   </si>
   <si>
-    <t>R7, R13, R16, R22, R45, R46, R52, R53, R64, R65, R73, R74, R79, R80, R83, R84, R94, R95, R104, R105</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -622,9 +619,6 @@
     <t>RC0402FR-07309KL</t>
   </si>
   <si>
-    <t>R25, R55, R87</t>
-  </si>
-  <si>
     <t>69.8k 1%</t>
   </si>
   <si>
@@ -646,9 +640,6 @@
     <t>RT0402BRD072KL</t>
   </si>
   <si>
-    <t>R27, R28, R56, R57, R89, R90</t>
-  </si>
-  <si>
     <t>182k 1%</t>
   </si>
   <si>
@@ -670,12 +661,6 @@
     <t>CRM2512-JW-1R0ELF</t>
   </si>
   <si>
-    <t>R76, R85, R100</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>R110</t>
   </si>
   <si>
@@ -968,12 +953,24 @@
   </si>
   <si>
     <t xml:space="preserve">U13, U16, U19, U22, U24, U27 </t>
+  </si>
+  <si>
+    <t>1R</t>
+  </si>
+  <si>
+    <t>R27, R28, R56, R57, R89, R90, R100</t>
+  </si>
+  <si>
+    <t>R25, R55, R85, R87</t>
+  </si>
+  <si>
+    <t>R7, R13, R16, R22, R45, R46, R52, R53, R64, R65, R73, R74, R76, R79, R80, R83, R84, R94, R95, R104, R105</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1460,9 +1457,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1817,16 +1820,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="32.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
@@ -1842,7 +1845,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1871,7 +1874,7 @@
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
@@ -1897,7 +1900,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
@@ -1916,14 +1919,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
@@ -1949,7 +1952,7 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
@@ -1962,23 +1965,23 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>101</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
@@ -2004,7 +2007,7 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
@@ -2030,7 +2033,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D9" t="s">
@@ -2056,7 +2059,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D10" t="s">
@@ -2082,7 +2085,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D11" t="s">
@@ -2108,7 +2111,7 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D12" t="s">
@@ -2134,7 +2137,7 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D13" t="s">
@@ -2160,7 +2163,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D14" t="s">
@@ -2186,7 +2189,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D15" t="s">
@@ -2205,14 +2208,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D16" t="s">
@@ -2238,7 +2241,7 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D17" t="s">
@@ -2264,7 +2267,7 @@
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D18" t="s">
@@ -2290,7 +2293,7 @@
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D19" t="s">
@@ -2316,7 +2319,7 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D20" t="s">
@@ -2342,7 +2345,7 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D21" t="s">
@@ -2368,7 +2371,7 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>87</v>
       </c>
       <c r="D22" t="s">
@@ -2394,7 +2397,7 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>91</v>
       </c>
       <c r="D23" t="s">
@@ -2420,7 +2423,7 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D24" t="s">
@@ -2446,7 +2449,7 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>100</v>
       </c>
       <c r="D25" t="s">
@@ -2472,7 +2475,7 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D26" t="s">
@@ -2498,7 +2501,7 @@
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>109</v>
       </c>
       <c r="D27" t="s">
@@ -2524,7 +2527,7 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D28" t="s">
@@ -2550,7 +2553,7 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>119</v>
       </c>
       <c r="D29" t="s">
@@ -2576,7 +2579,7 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D30" t="s">
@@ -2602,7 +2605,7 @@
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>128</v>
       </c>
       <c r="D31" t="s">
@@ -2628,7 +2631,7 @@
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D32" t="s">
@@ -2654,7 +2657,7 @@
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D33" t="s">
@@ -2680,11 +2683,11 @@
       <c r="B34">
         <v>5</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E34" t="s">
         <v>144</v>
@@ -2706,7 +2709,7 @@
       <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D35" t="s">
@@ -2732,7 +2735,7 @@
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="3" t="s">
         <v>151</v>
       </c>
       <c r="D36" t="s">
@@ -2758,7 +2761,7 @@
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D37" t="s">
@@ -2777,27 +2780,27 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>20</v>
-      </c>
-      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D38" t="s">
         <v>159</v>
-      </c>
-      <c r="D38" t="s">
-        <v>160</v>
       </c>
       <c r="E38" t="s">
         <v>144</v>
       </c>
       <c r="G38" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" t="s">
         <v>161</v>
-      </c>
-      <c r="H38" t="s">
-        <v>162</v>
       </c>
       <c r="I38" t="s">
         <v>142</v>
@@ -2810,20 +2813,20 @@
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" t="s">
         <v>163</v>
-      </c>
-      <c r="D39" t="s">
-        <v>164</v>
       </c>
       <c r="E39" t="s">
         <v>144</v>
       </c>
       <c r="G39" t="s">
+        <v>164</v>
+      </c>
+      <c r="H39" t="s">
         <v>165</v>
-      </c>
-      <c r="H39" t="s">
-        <v>166</v>
       </c>
       <c r="I39" t="s">
         <v>142</v>
@@ -2836,20 +2839,20 @@
       <c r="B40">
         <v>2</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" t="s">
         <v>167</v>
-      </c>
-      <c r="D40" t="s">
-        <v>168</v>
       </c>
       <c r="E40" t="s">
         <v>144</v>
       </c>
       <c r="G40" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" t="s">
         <v>169</v>
-      </c>
-      <c r="H40" t="s">
-        <v>170</v>
       </c>
       <c r="I40" t="s">
         <v>142</v>
@@ -2862,20 +2865,20 @@
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" t="s">
         <v>171</v>
-      </c>
-      <c r="D41" t="s">
-        <v>172</v>
       </c>
       <c r="E41" t="s">
         <v>144</v>
       </c>
       <c r="G41" t="s">
+        <v>172</v>
+      </c>
+      <c r="H41" t="s">
         <v>173</v>
-      </c>
-      <c r="H41" t="s">
-        <v>174</v>
       </c>
       <c r="I41" t="s">
         <v>142</v>
@@ -2888,8 +2891,8 @@
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" t="s">
-        <v>175</v>
+      <c r="C42" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
@@ -2911,72 +2914,72 @@
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" t="s">
         <v>176</v>
-      </c>
-      <c r="D43" t="s">
-        <v>177</v>
       </c>
       <c r="E43" t="s">
         <v>144</v>
       </c>
       <c r="G43" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" t="s">
         <v>178</v>
-      </c>
-      <c r="H43" t="s">
-        <v>179</v>
       </c>
       <c r="I43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
         <v>19</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" t="s">
         <v>180</v>
-      </c>
-      <c r="D44" t="s">
-        <v>181</v>
       </c>
       <c r="E44" t="s">
         <v>144</v>
       </c>
       <c r="G44" t="s">
+        <v>181</v>
+      </c>
+      <c r="H44" t="s">
         <v>182</v>
-      </c>
-      <c r="H44" t="s">
-        <v>183</v>
       </c>
       <c r="I44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
         <v>20</v>
       </c>
-      <c r="C45" t="s">
-        <v>184</v>
+      <c r="C45" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="D45" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E45" t="s">
         <v>144</v>
       </c>
       <c r="G45" t="s">
+        <v>184</v>
+      </c>
+      <c r="H45" t="s">
         <v>185</v>
-      </c>
-      <c r="H45" t="s">
-        <v>186</v>
       </c>
       <c r="I45" t="s">
         <v>142</v>
@@ -2989,20 +2992,20 @@
       <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" t="s">
         <v>187</v>
-      </c>
-      <c r="D46" t="s">
-        <v>188</v>
       </c>
       <c r="E46" t="s">
         <v>144</v>
       </c>
       <c r="G46" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" t="s">
         <v>189</v>
-      </c>
-      <c r="H46" t="s">
-        <v>190</v>
       </c>
       <c r="I46" t="s">
         <v>142</v>
@@ -3015,20 +3018,20 @@
       <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" t="s">
         <v>191</v>
-      </c>
-      <c r="D47" t="s">
-        <v>192</v>
       </c>
       <c r="E47" t="s">
         <v>144</v>
       </c>
       <c r="G47" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" t="s">
         <v>193</v>
-      </c>
-      <c r="H47" t="s">
-        <v>194</v>
       </c>
       <c r="I47" t="s">
         <v>142</v>
@@ -3041,11 +3044,11 @@
       <c r="B48">
         <v>6</v>
       </c>
-      <c r="C48" t="s">
-        <v>195</v>
+      <c r="C48" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D48" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E48" t="s">
         <v>144</v>
@@ -3054,7 +3057,7 @@
         <v>5</v>
       </c>
       <c r="H48" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="I48" t="s">
         <v>142</v>
@@ -3067,20 +3070,20 @@
       <c r="B49">
         <v>3</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D49" t="s">
         <v>196</v>
-      </c>
-      <c r="D49" t="s">
-        <v>197</v>
       </c>
       <c r="E49" t="s">
         <v>144</v>
       </c>
       <c r="G49" t="s">
+        <v>197</v>
+      </c>
+      <c r="H49" t="s">
         <v>198</v>
-      </c>
-      <c r="H49" t="s">
-        <v>199</v>
       </c>
       <c r="I49" t="s">
         <v>142</v>
@@ -3091,22 +3094,22 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>200</v>
+        <v>4</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>313</v>
       </c>
       <c r="D50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E50" t="s">
         <v>144</v>
       </c>
       <c r="G50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I50" t="s">
         <v>142</v>
@@ -3119,20 +3122,20 @@
       <c r="B51">
         <v>3</v>
       </c>
-      <c r="C51" t="s">
-        <v>204</v>
+      <c r="C51" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D51" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E51" t="s">
         <v>144</v>
       </c>
       <c r="G51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H51" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I51" t="s">
         <v>142</v>
@@ -3143,22 +3146,22 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>6</v>
-      </c>
-      <c r="C52" t="s">
-        <v>208</v>
+        <v>7</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>312</v>
       </c>
       <c r="D52" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E52" t="s">
         <v>144</v>
       </c>
       <c r="G52" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H52" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I52" t="s">
         <v>142</v>
@@ -3171,20 +3174,20 @@
       <c r="B53">
         <v>6</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" t="s">
+        <v>311</v>
+      </c>
+      <c r="E53" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" t="s">
+        <v>211</v>
+      </c>
+      <c r="H53" t="s">
         <v>212</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>213</v>
-      </c>
-      <c r="G53" t="s">
-        <v>214</v>
-      </c>
-      <c r="H53" t="s">
-        <v>215</v>
       </c>
       <c r="I53" t="s">
         <v>142</v>
@@ -3195,22 +3198,22 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>216</v>
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
         <v>144</v>
       </c>
       <c r="G54" t="s">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="H54" t="s">
-        <v>162</v>
+        <v>216</v>
       </c>
       <c r="I54" t="s">
         <v>142</v>
@@ -3223,20 +3226,20 @@
       <c r="B55">
         <v>1</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" t="s">
         <v>218</v>
-      </c>
-      <c r="D55" t="s">
-        <v>219</v>
       </c>
       <c r="E55" t="s">
         <v>144</v>
       </c>
       <c r="G55" t="s">
+        <v>219</v>
+      </c>
+      <c r="H55" t="s">
         <v>220</v>
-      </c>
-      <c r="H55" t="s">
-        <v>221</v>
       </c>
       <c r="I55" t="s">
         <v>142</v>
@@ -3249,20 +3252,20 @@
       <c r="B56">
         <v>1</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" t="s">
         <v>222</v>
-      </c>
-      <c r="D56" t="s">
-        <v>223</v>
       </c>
       <c r="E56" t="s">
         <v>144</v>
       </c>
       <c r="G56" t="s">
-        <v>224</v>
+        <v>308</v>
       </c>
       <c r="H56" t="s">
-        <v>225</v>
+        <v>309</v>
       </c>
       <c r="I56" t="s">
         <v>142</v>
@@ -3275,20 +3278,20 @@
       <c r="B57">
         <v>1</v>
       </c>
-      <c r="C57" t="s">
-        <v>226</v>
+      <c r="C57" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="D57" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E57" t="s">
         <v>144</v>
       </c>
       <c r="G57" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="H57" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I57" t="s">
         <v>142</v>
@@ -3299,25 +3302,25 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
+        <v>227</v>
+      </c>
+      <c r="G58" t="s">
         <v>228</v>
       </c>
-      <c r="D58" t="s">
+      <c r="H58" t="s">
+        <v>226</v>
+      </c>
+      <c r="I58" t="s">
         <v>229</v>
-      </c>
-      <c r="E58" t="s">
-        <v>144</v>
-      </c>
-      <c r="G58" t="s">
-        <v>312</v>
-      </c>
-      <c r="H58" t="s">
-        <v>311</v>
-      </c>
-      <c r="I58" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3325,9 +3328,9 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>230</v>
       </c>
       <c r="D59" t="s">
@@ -3340,10 +3343,10 @@
         <v>233</v>
       </c>
       <c r="H59" t="s">
+        <v>234</v>
+      </c>
+      <c r="I59" t="s">
         <v>231</v>
-      </c>
-      <c r="I59" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3353,7 +3356,7 @@
       <c r="B60">
         <v>1</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="3" t="s">
         <v>235</v>
       </c>
       <c r="D60" t="s">
@@ -3366,7 +3369,7 @@
         <v>238</v>
       </c>
       <c r="H60" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I60" t="s">
         <v>236</v>
@@ -3379,23 +3382,23 @@
       <c r="B61">
         <v>1</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D61" t="s">
         <v>240</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>241</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>242</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I61" t="s">
         <v>243</v>
-      </c>
-      <c r="H61" t="s">
-        <v>241</v>
-      </c>
-      <c r="I61" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3405,7 +3408,7 @@
       <c r="B62">
         <v>1</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>244</v>
       </c>
       <c r="D62" t="s">
@@ -3418,10 +3421,10 @@
         <v>247</v>
       </c>
       <c r="H62" t="s">
+        <v>248</v>
+      </c>
+      <c r="I62" t="s">
         <v>245</v>
-      </c>
-      <c r="I62" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3431,7 +3434,7 @@
       <c r="B63">
         <v>1</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
         <v>249</v>
       </c>
       <c r="D63" t="s">
@@ -3457,7 +3460,7 @@
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
         <v>254</v>
       </c>
       <c r="D64" t="s">
@@ -3470,7 +3473,7 @@
         <v>257</v>
       </c>
       <c r="H64" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I64" t="s">
         <v>255</v>
@@ -3483,23 +3486,23 @@
       <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D65" t="s">
         <v>259</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>260</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>261</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>262</v>
       </c>
-      <c r="H65" t="s">
-        <v>260</v>
-      </c>
       <c r="I65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3507,9 +3510,9 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>263</v>
       </c>
       <c r="D66" t="s">
@@ -3525,7 +3528,7 @@
         <v>267</v>
       </c>
       <c r="I66" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3533,25 +3536,25 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>3</v>
-      </c>
-      <c r="C67" t="s">
-        <v>268</v>
+        <v>1</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="D67" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E67" t="s">
+        <v>271</v>
+      </c>
+      <c r="G67" t="s">
+        <v>272</v>
+      </c>
+      <c r="H67" t="s">
+        <v>273</v>
+      </c>
+      <c r="I67" t="s">
         <v>270</v>
-      </c>
-      <c r="G67" t="s">
-        <v>271</v>
-      </c>
-      <c r="H67" t="s">
-        <v>272</v>
-      </c>
-      <c r="I67" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3561,7 +3564,7 @@
       <c r="B68">
         <v>1</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="3" t="s">
         <v>274</v>
       </c>
       <c r="D68" t="s">
@@ -3587,23 +3590,23 @@
       <c r="B69">
         <v>1</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="3" t="s">
         <v>279</v>
       </c>
       <c r="D69" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E69" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G69" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H69" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I69" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3613,23 +3616,23 @@
       <c r="B70">
         <v>1</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D70" t="s">
+        <v>281</v>
+      </c>
+      <c r="E70" t="s">
+        <v>282</v>
+      </c>
+      <c r="G70" t="s">
+        <v>283</v>
+      </c>
+      <c r="H70" t="s">
         <v>284</v>
       </c>
-      <c r="D70" t="s">
-        <v>280</v>
-      </c>
-      <c r="E70" t="s">
-        <v>281</v>
-      </c>
-      <c r="G70" t="s">
-        <v>282</v>
-      </c>
-      <c r="H70" t="s">
-        <v>283</v>
-      </c>
       <c r="I70" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3637,25 +3640,19 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D71" t="s">
         <v>285</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>286</v>
       </c>
-      <c r="E71" t="s">
-        <v>287</v>
-      </c>
-      <c r="G71" t="s">
-        <v>288</v>
-      </c>
-      <c r="H71" t="s">
-        <v>289</v>
-      </c>
       <c r="I71" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3665,17 +3662,23 @@
       <c r="B72">
         <v>6</v>
       </c>
-      <c r="C72" t="s">
-        <v>315</v>
+      <c r="C72" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="D72" t="s">
+        <v>288</v>
+      </c>
+      <c r="E72" t="s">
+        <v>289</v>
+      </c>
+      <c r="G72" t="s">
         <v>290</v>
       </c>
-      <c r="E72" t="s">
+      <c r="H72" t="s">
         <v>291</v>
       </c>
       <c r="I72" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3683,9 +3686,9 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>6</v>
-      </c>
-      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>292</v>
       </c>
       <c r="D73" t="s">
@@ -3709,9 +3712,9 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>2</v>
-      </c>
-      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>297</v>
       </c>
       <c r="D74" t="s">
@@ -3727,33 +3730,7 @@
         <v>301</v>
       </c>
       <c r="I74" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>73</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
         <v>302</v>
-      </c>
-      <c r="D75" t="s">
-        <v>303</v>
-      </c>
-      <c r="E75" t="s">
-        <v>304</v>
-      </c>
-      <c r="G75" t="s">
-        <v>305</v>
-      </c>
-      <c r="H75" t="s">
-        <v>306</v>
-      </c>
-      <c r="I75" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add updated BOM and new gerber files for v301
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-301-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-301-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F427C4-9489-40B0-BC3A-032888E061ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274C3092-0DA1-4603-A67C-B5FCE489E3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30135" yWindow="1155" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="313">
   <si>
     <t>Item</t>
   </si>
@@ -301,27 +301,12 @@
     <t>Screw Terminal</t>
   </si>
   <si>
-    <t>bitaxe:7770-screw-terminal</t>
-  </si>
-  <si>
-    <t>36-7770-ND</t>
-  </si>
-  <si>
-    <t>36-7770</t>
-  </si>
-  <si>
     <t>Conn_01x01</t>
   </si>
   <si>
     <t>J2</t>
   </si>
   <si>
-    <t>A100886CT-ND</t>
-  </si>
-  <si>
-    <t>63862-1</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -965,6 +950,15 @@
   </si>
   <si>
     <t>R7, R13, R16, R22, R45, R46, R52, R53, R64, R65, R73, R74, R76, R79, R80, R83, R84, R94, R95, R104, R105</t>
+  </si>
+  <si>
+    <t>bitaxe:7771-screw-terminal</t>
+  </si>
+  <si>
+    <t>36-7771-ND</t>
+  </si>
+  <si>
+    <t>36-7771</t>
   </si>
 </sst>
 </file>
@@ -1823,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,10 +1959,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -2404,16 +2398,16 @@
         <v>92</v>
       </c>
       <c r="E23" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" t="s">
+        <v>311</v>
+      </c>
+      <c r="H23" t="s">
+        <v>312</v>
+      </c>
+      <c r="I23" t="s">
         <v>93</v>
-      </c>
-      <c r="G23" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2424,22 +2418,22 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E24" t="s">
+        <v>310</v>
+      </c>
+      <c r="G24" t="s">
+        <v>311</v>
+      </c>
+      <c r="H24" t="s">
+        <v>312</v>
+      </c>
+      <c r="I24" t="s">
         <v>93</v>
-      </c>
-      <c r="G24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" t="s">
-        <v>99</v>
-      </c>
-      <c r="I24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2450,22 +2444,22 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2476,22 +2470,22 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H26">
         <v>470531000</v>
       </c>
       <c r="I26" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2502,22 +2496,22 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I27" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,22 +2522,22 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H28">
         <v>744373580047</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2554,22 +2548,22 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E29" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G29" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H29">
         <v>74438357082</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2580,22 +2574,22 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I30" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2606,22 +2600,22 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" t="s">
         <v>125</v>
       </c>
-      <c r="G31" t="s">
-        <v>130</v>
-      </c>
       <c r="H31" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I31" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2632,22 +2626,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G32" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H32" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I32" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2658,22 +2652,22 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" t="s">
         <v>137</v>
-      </c>
-      <c r="D33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" t="s">
-        <v>139</v>
-      </c>
-      <c r="G33" t="s">
-        <v>140</v>
-      </c>
-      <c r="H33" t="s">
-        <v>141</v>
-      </c>
-      <c r="I33" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2684,22 +2678,22 @@
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G34" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H34" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I34" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2710,22 +2704,22 @@
         <v>2</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" t="s">
         <v>144</v>
       </c>
-      <c r="G35" t="s">
-        <v>149</v>
-      </c>
       <c r="H35" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2736,22 +2730,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G36" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I36" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2762,22 +2756,22 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I37" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2788,22 +2782,22 @@
         <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I38" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2814,22 +2808,22 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E39" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G39" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H39" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I39" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2840,22 +2834,22 @@
         <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E40" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G40" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H40" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2866,22 +2860,22 @@
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G41" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H41" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2892,19 +2886,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
       </c>
       <c r="I42" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2915,22 +2909,22 @@
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D43" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E43" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G43" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H43" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I43" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2941,22 +2935,22 @@
         <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E44" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G44" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H44" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I44" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2967,22 +2961,22 @@
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D45" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E45" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G45" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H45" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I45" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2993,22 +2987,22 @@
         <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G46" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H46" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I46" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3019,22 +3013,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D47" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G47" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H47" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I47" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3045,22 +3039,22 @@
         <v>6</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D48" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E48" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F48" t="s">
         <v>5</v>
       </c>
       <c r="H48" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I48" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3071,22 +3065,22 @@
         <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G49" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H49" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I49" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3097,22 +3091,22 @@
         <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E50" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H50" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I50" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3123,22 +3117,22 @@
         <v>3</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D51" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G51" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H51" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I51" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3149,22 +3143,22 @@
         <v>7</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E52" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G52" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H52" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I52" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3175,22 +3169,22 @@
         <v>6</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D53" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E53" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G53" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H53" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I53" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3201,22 +3195,22 @@
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D54" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G54" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H54" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I54" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3227,22 +3221,22 @@
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D55" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G55" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H55" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I55" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3253,22 +3247,22 @@
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D56" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E56" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G56" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H56" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I56" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3279,22 +3273,22 @@
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D57" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G57" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H57" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I57" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3305,22 +3299,22 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D58" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E58" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G58" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H58" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I58" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3331,22 +3325,22 @@
         <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D59" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G59" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H59" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I59" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3357,22 +3351,22 @@
         <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G60" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H60" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I60" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3383,22 +3377,22 @@
         <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D61" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E61" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G61" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H61" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I61" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3409,22 +3403,22 @@
         <v>1</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E62" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G62" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H62" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I62" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3435,22 +3429,22 @@
         <v>1</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D63" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E63" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G63" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H63" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I63" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3461,22 +3455,22 @@
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D64" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E64" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G64" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H64" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I64" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3487,22 +3481,22 @@
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D65" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E65" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G65" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H65" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="I65" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3513,22 +3507,22 @@
         <v>3</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D66" t="s">
+        <v>259</v>
+      </c>
+      <c r="E66" t="s">
+        <v>260</v>
+      </c>
+      <c r="G66" t="s">
+        <v>261</v>
+      </c>
+      <c r="H66" t="s">
+        <v>262</v>
+      </c>
+      <c r="I66" t="s">
         <v>263</v>
-      </c>
-      <c r="D66" t="s">
-        <v>264</v>
-      </c>
-      <c r="E66" t="s">
-        <v>265</v>
-      </c>
-      <c r="G66" t="s">
-        <v>266</v>
-      </c>
-      <c r="H66" t="s">
-        <v>267</v>
-      </c>
-      <c r="I66" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3539,22 +3533,22 @@
         <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D67" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E67" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="G67" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H67" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I67" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3565,22 +3559,22 @@
         <v>1</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D68" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E68" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G68" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H68" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I68" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3591,22 +3585,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D69" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E69" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G69" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H69" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I69" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3617,22 +3611,22 @@
         <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D70" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E70" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G70" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H70" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I70" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3643,16 +3637,16 @@
         <v>6</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D71" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E71" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I71" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3663,22 +3657,22 @@
         <v>6</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D72" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E72" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G72" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H72" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I72" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3689,22 +3683,22 @@
         <v>2</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D73" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E73" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G73" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H73" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I73" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3715,22 +3709,22 @@
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D74" t="s">
+        <v>293</v>
+      </c>
+      <c r="E74" t="s">
+        <v>294</v>
+      </c>
+      <c r="G74" t="s">
+        <v>295</v>
+      </c>
+      <c r="H74" t="s">
+        <v>296</v>
+      </c>
+      <c r="I74" t="s">
         <v>297</v>
-      </c>
-      <c r="D74" t="s">
-        <v>298</v>
-      </c>
-      <c r="E74" t="s">
-        <v>299</v>
-      </c>
-      <c r="G74" t="s">
-        <v>300</v>
-      </c>
-      <c r="H74" t="s">
-        <v>301</v>
-      </c>
-      <c r="I74" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust some values on the BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeHex-301-BOM.xlsx
+++ b/Manufacturing Files/bitaxeHex-301-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\bitaxeHex\Manufacturing Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274C3092-0DA1-4603-A67C-B5FCE489E3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128A2E3F-46B9-4AE7-B63B-9608AF54B33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30135" yWindow="1155" windowWidth="24165" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="1005" windowWidth="24165" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bitaxeHex" sheetId="1" r:id="rId1"/>
@@ -373,9 +373,6 @@
     <t>bitaxe:74438357082</t>
   </si>
   <si>
-    <t>732-11205-1-ND</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -478,12 +475,6 @@
     <t>3.83K</t>
   </si>
   <si>
-    <t>311-1.33KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-071K33L</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -959,6 +950,15 @@
   </si>
   <si>
     <t>36-7771</t>
+  </si>
+  <si>
+    <t>732-11745-1-ND</t>
+  </si>
+  <si>
+    <t>311-3.83KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-073K83L</t>
   </si>
 </sst>
 </file>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,10 +1959,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
@@ -2398,13 +2398,13 @@
         <v>92</v>
       </c>
       <c r="E23" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G23" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H23" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="I23" t="s">
         <v>93</v>
@@ -2424,13 +2424,13 @@
         <v>92</v>
       </c>
       <c r="E24" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G24" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H24" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="I24" t="s">
         <v>93</v>
@@ -2557,10 +2557,10 @@
         <v>116</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>310</v>
       </c>
       <c r="H29">
-        <v>74438357082</v>
+        <v>78438357082</v>
       </c>
       <c r="I29" t="s">
         <v>113</v>
@@ -2574,22 +2574,22 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" t="s">
         <v>118</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>119</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>120</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" t="s">
         <v>121</v>
-      </c>
-      <c r="H30" t="s">
-        <v>119</v>
-      </c>
-      <c r="I30" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2600,22 +2600,22 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
         <v>123</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
+      <c r="G31" t="s">
         <v>124</v>
       </c>
-      <c r="E31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" t="s">
         <v>125</v>
-      </c>
-      <c r="H31" t="s">
-        <v>124</v>
-      </c>
-      <c r="I31" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2626,22 +2626,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s">
         <v>127</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>128</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>129</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>130</v>
       </c>
-      <c r="H32" t="s">
-        <v>131</v>
-      </c>
       <c r="I32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2652,22 +2652,22 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
         <v>132</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>133</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>134</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>135</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>136</v>
-      </c>
-      <c r="I33" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2678,22 +2678,22 @@
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>296</v>
+      </c>
+      <c r="E34" t="s">
         <v>138</v>
       </c>
-      <c r="D34" t="s">
-        <v>299</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>139</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>140</v>
       </c>
-      <c r="H34" t="s">
-        <v>141</v>
-      </c>
       <c r="I34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2704,22 +2704,22 @@
         <v>2</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" t="s">
         <v>143</v>
       </c>
-      <c r="E35" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>144</v>
       </c>
-      <c r="H35" t="s">
-        <v>145</v>
-      </c>
       <c r="I35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2730,22 +2730,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" t="s">
         <v>146</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" t="s">
         <v>147</v>
       </c>
-      <c r="E36" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>148</v>
       </c>
-      <c r="H36" t="s">
-        <v>149</v>
-      </c>
       <c r="I36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2756,22 +2756,22 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
         <v>150</v>
       </c>
-      <c r="D37" t="s">
-        <v>151</v>
-      </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>311</v>
       </c>
       <c r="H37" t="s">
-        <v>153</v>
+        <v>312</v>
       </c>
       <c r="I37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2782,22 +2782,22 @@
         <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2808,22 +2808,22 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" t="s">
         <v>157</v>
       </c>
-      <c r="D39" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G39" t="s">
-        <v>159</v>
-      </c>
-      <c r="H39" t="s">
-        <v>160</v>
-      </c>
       <c r="I39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2834,22 +2834,22 @@
         <v>2</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" t="s">
+        <v>160</v>
+      </c>
+      <c r="H40" t="s">
         <v>161</v>
       </c>
-      <c r="D40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E40" t="s">
-        <v>139</v>
-      </c>
-      <c r="G40" t="s">
-        <v>163</v>
-      </c>
-      <c r="H40" t="s">
-        <v>164</v>
-      </c>
       <c r="I40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2860,22 +2860,22 @@
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" t="s">
+        <v>164</v>
+      </c>
+      <c r="H41" t="s">
         <v>165</v>
       </c>
-      <c r="D41" t="s">
-        <v>166</v>
-      </c>
-      <c r="E41" t="s">
-        <v>139</v>
-      </c>
-      <c r="G41" t="s">
-        <v>167</v>
-      </c>
-      <c r="H41" t="s">
-        <v>168</v>
-      </c>
       <c r="I41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2886,19 +2886,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
       </c>
       <c r="I42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2909,22 +2909,22 @@
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" t="s">
         <v>170</v>
       </c>
-      <c r="D43" t="s">
-        <v>171</v>
-      </c>
-      <c r="E43" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" t="s">
-        <v>172</v>
-      </c>
-      <c r="H43" t="s">
-        <v>173</v>
-      </c>
       <c r="I43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2935,22 +2935,22 @@
         <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" t="s">
+        <v>173</v>
+      </c>
+      <c r="H44" t="s">
         <v>174</v>
       </c>
-      <c r="D44" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G44" t="s">
-        <v>176</v>
-      </c>
-      <c r="H44" t="s">
-        <v>177</v>
-      </c>
       <c r="I44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2961,22 +2961,22 @@
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D45" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G45" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H45" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2987,22 +2987,22 @@
         <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" t="s">
+        <v>180</v>
+      </c>
+      <c r="H46" t="s">
         <v>181</v>
       </c>
-      <c r="D46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" t="s">
-        <v>183</v>
-      </c>
-      <c r="H46" t="s">
-        <v>184</v>
-      </c>
       <c r="I46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3013,22 +3013,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" t="s">
+        <v>183</v>
+      </c>
+      <c r="E47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" t="s">
+        <v>184</v>
+      </c>
+      <c r="H47" t="s">
         <v>185</v>
       </c>
-      <c r="D47" t="s">
-        <v>186</v>
-      </c>
-      <c r="E47" t="s">
-        <v>139</v>
-      </c>
-      <c r="G47" t="s">
-        <v>187</v>
-      </c>
-      <c r="H47" t="s">
-        <v>188</v>
-      </c>
       <c r="I47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3039,22 +3039,22 @@
         <v>6</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D48" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
         <v>5</v>
       </c>
       <c r="H48" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3065,22 +3065,22 @@
         <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" t="s">
+        <v>138</v>
+      </c>
+      <c r="G49" t="s">
+        <v>189</v>
+      </c>
+      <c r="H49" t="s">
         <v>190</v>
       </c>
-      <c r="D49" t="s">
-        <v>191</v>
-      </c>
-      <c r="E49" t="s">
-        <v>139</v>
-      </c>
-      <c r="G49" t="s">
-        <v>192</v>
-      </c>
-      <c r="H49" t="s">
-        <v>193</v>
-      </c>
       <c r="I49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3091,22 +3091,22 @@
         <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H50" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3117,22 +3117,22 @@
         <v>3</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D51" t="s">
+        <v>195</v>
+      </c>
+      <c r="E51" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" t="s">
+        <v>196</v>
+      </c>
+      <c r="H51" t="s">
         <v>197</v>
       </c>
-      <c r="D51" t="s">
-        <v>198</v>
-      </c>
-      <c r="E51" t="s">
-        <v>139</v>
-      </c>
-      <c r="G51" t="s">
-        <v>199</v>
-      </c>
-      <c r="H51" t="s">
-        <v>200</v>
-      </c>
       <c r="I51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3143,22 +3143,22 @@
         <v>7</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H52" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3169,22 +3169,22 @@
         <v>6</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D53" t="s">
+        <v>303</v>
+      </c>
+      <c r="E53" t="s">
+        <v>202</v>
+      </c>
+      <c r="G53" t="s">
+        <v>203</v>
+      </c>
+      <c r="H53" t="s">
         <v>204</v>
       </c>
-      <c r="D53" t="s">
-        <v>306</v>
-      </c>
-      <c r="E53" t="s">
-        <v>205</v>
-      </c>
-      <c r="G53" t="s">
-        <v>206</v>
-      </c>
-      <c r="H53" t="s">
-        <v>207</v>
-      </c>
       <c r="I53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3195,22 +3195,22 @@
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" t="s">
+        <v>138</v>
+      </c>
+      <c r="G54" t="s">
+        <v>207</v>
+      </c>
+      <c r="H54" t="s">
         <v>208</v>
       </c>
-      <c r="D54" t="s">
-        <v>209</v>
-      </c>
-      <c r="E54" t="s">
-        <v>139</v>
-      </c>
-      <c r="G54" t="s">
-        <v>210</v>
-      </c>
-      <c r="H54" t="s">
-        <v>211</v>
-      </c>
       <c r="I54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3221,22 +3221,22 @@
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D55" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" t="s">
+        <v>211</v>
+      </c>
+      <c r="H55" t="s">
         <v>212</v>
       </c>
-      <c r="D55" t="s">
-        <v>213</v>
-      </c>
-      <c r="E55" t="s">
-        <v>139</v>
-      </c>
-      <c r="G55" t="s">
-        <v>214</v>
-      </c>
-      <c r="H55" t="s">
-        <v>215</v>
-      </c>
       <c r="I55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3247,22 +3247,22 @@
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G56" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H56" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3273,22 +3273,22 @@
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D57" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G57" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H57" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3299,22 +3299,22 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D58" t="s">
+        <v>218</v>
+      </c>
+      <c r="E58" t="s">
+        <v>219</v>
+      </c>
+      <c r="G58" t="s">
         <v>220</v>
       </c>
-      <c r="D58" t="s">
+      <c r="H58" t="s">
+        <v>218</v>
+      </c>
+      <c r="I58" t="s">
         <v>221</v>
-      </c>
-      <c r="E58" t="s">
-        <v>222</v>
-      </c>
-      <c r="G58" t="s">
-        <v>223</v>
-      </c>
-      <c r="H58" t="s">
-        <v>221</v>
-      </c>
-      <c r="I58" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3325,22 +3325,22 @@
         <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D59" t="s">
+        <v>223</v>
+      </c>
+      <c r="E59" t="s">
+        <v>224</v>
+      </c>
+      <c r="G59" t="s">
         <v>225</v>
       </c>
-      <c r="D59" t="s">
+      <c r="H59" t="s">
         <v>226</v>
       </c>
-      <c r="E59" t="s">
-        <v>227</v>
-      </c>
-      <c r="G59" t="s">
-        <v>228</v>
-      </c>
-      <c r="H59" t="s">
-        <v>229</v>
-      </c>
       <c r="I59" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3351,22 +3351,22 @@
         <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" t="s">
+        <v>228</v>
+      </c>
+      <c r="E60" t="s">
+        <v>229</v>
+      </c>
+      <c r="G60" t="s">
         <v>230</v>
       </c>
-      <c r="D60" t="s">
-        <v>231</v>
-      </c>
-      <c r="E60" t="s">
-        <v>232</v>
-      </c>
-      <c r="G60" t="s">
-        <v>233</v>
-      </c>
       <c r="H60" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I60" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3377,22 +3377,22 @@
         <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D61" t="s">
+        <v>232</v>
+      </c>
+      <c r="E61" t="s">
+        <v>233</v>
+      </c>
+      <c r="G61" t="s">
         <v>234</v>
       </c>
-      <c r="D61" t="s">
+      <c r="H61" t="s">
+        <v>232</v>
+      </c>
+      <c r="I61" t="s">
         <v>235</v>
-      </c>
-      <c r="E61" t="s">
-        <v>236</v>
-      </c>
-      <c r="G61" t="s">
-        <v>237</v>
-      </c>
-      <c r="H61" t="s">
-        <v>235</v>
-      </c>
-      <c r="I61" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3403,22 +3403,22 @@
         <v>1</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" t="s">
+        <v>237</v>
+      </c>
+      <c r="E62" t="s">
+        <v>238</v>
+      </c>
+      <c r="G62" t="s">
         <v>239</v>
       </c>
-      <c r="D62" t="s">
+      <c r="H62" t="s">
         <v>240</v>
       </c>
-      <c r="E62" t="s">
-        <v>241</v>
-      </c>
-      <c r="G62" t="s">
-        <v>242</v>
-      </c>
-      <c r="H62" t="s">
-        <v>243</v>
-      </c>
       <c r="I62" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3429,22 +3429,22 @@
         <v>1</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D63" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" t="s">
+        <v>243</v>
+      </c>
+      <c r="G63" t="s">
         <v>244</v>
       </c>
-      <c r="D63" t="s">
+      <c r="H63" t="s">
         <v>245</v>
       </c>
-      <c r="E63" t="s">
-        <v>246</v>
-      </c>
-      <c r="G63" t="s">
-        <v>247</v>
-      </c>
-      <c r="H63" t="s">
-        <v>248</v>
-      </c>
       <c r="I63" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3455,22 +3455,22 @@
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D64" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" t="s">
+        <v>248</v>
+      </c>
+      <c r="G64" t="s">
         <v>249</v>
       </c>
-      <c r="D64" t="s">
-        <v>250</v>
-      </c>
-      <c r="E64" t="s">
-        <v>251</v>
-      </c>
-      <c r="G64" t="s">
-        <v>252</v>
-      </c>
       <c r="H64" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="I64" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3481,22 +3481,22 @@
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D65" t="s">
+        <v>251</v>
+      </c>
+      <c r="E65" t="s">
+        <v>252</v>
+      </c>
+      <c r="G65" t="s">
         <v>253</v>
       </c>
-      <c r="D65" t="s">
+      <c r="H65" t="s">
         <v>254</v>
       </c>
-      <c r="E65" t="s">
-        <v>255</v>
-      </c>
-      <c r="G65" t="s">
-        <v>256</v>
-      </c>
-      <c r="H65" t="s">
-        <v>257</v>
-      </c>
       <c r="I65" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3507,22 +3507,22 @@
         <v>3</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D66" t="s">
+        <v>256</v>
+      </c>
+      <c r="E66" t="s">
+        <v>257</v>
+      </c>
+      <c r="G66" t="s">
         <v>258</v>
       </c>
-      <c r="D66" t="s">
+      <c r="H66" t="s">
         <v>259</v>
       </c>
-      <c r="E66" t="s">
+      <c r="I66" t="s">
         <v>260</v>
-      </c>
-      <c r="G66" t="s">
-        <v>261</v>
-      </c>
-      <c r="H66" t="s">
-        <v>262</v>
-      </c>
-      <c r="I66" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3533,22 +3533,22 @@
         <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D67" t="s">
+        <v>262</v>
+      </c>
+      <c r="E67" t="s">
+        <v>263</v>
+      </c>
+      <c r="G67" t="s">
         <v>264</v>
       </c>
-      <c r="D67" t="s">
+      <c r="H67" t="s">
         <v>265</v>
       </c>
-      <c r="E67" t="s">
-        <v>266</v>
-      </c>
-      <c r="G67" t="s">
-        <v>267</v>
-      </c>
-      <c r="H67" t="s">
-        <v>268</v>
-      </c>
       <c r="I67" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3559,22 +3559,22 @@
         <v>1</v>
       </c>
       <c r="C68" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D68" t="s">
+        <v>267</v>
+      </c>
+      <c r="E68" t="s">
+        <v>268</v>
+      </c>
+      <c r="G68" t="s">
         <v>269</v>
       </c>
-      <c r="D68" t="s">
+      <c r="H68" t="s">
         <v>270</v>
       </c>
-      <c r="E68" t="s">
-        <v>271</v>
-      </c>
-      <c r="G68" t="s">
-        <v>272</v>
-      </c>
-      <c r="H68" t="s">
-        <v>273</v>
-      </c>
       <c r="I68" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3585,22 +3585,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D69" t="s">
+        <v>267</v>
+      </c>
+      <c r="E69" t="s">
+        <v>268</v>
+      </c>
+      <c r="G69" t="s">
+        <v>269</v>
+      </c>
+      <c r="H69" t="s">
         <v>270</v>
       </c>
-      <c r="E69" t="s">
-        <v>271</v>
-      </c>
-      <c r="G69" t="s">
-        <v>272</v>
-      </c>
-      <c r="H69" t="s">
-        <v>273</v>
-      </c>
       <c r="I69" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3611,22 +3611,22 @@
         <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D70" t="s">
+        <v>273</v>
+      </c>
+      <c r="E70" t="s">
+        <v>274</v>
+      </c>
+      <c r="G70" t="s">
         <v>275</v>
       </c>
-      <c r="D70" t="s">
+      <c r="H70" t="s">
         <v>276</v>
       </c>
-      <c r="E70" t="s">
-        <v>277</v>
-      </c>
-      <c r="G70" t="s">
-        <v>278</v>
-      </c>
-      <c r="H70" t="s">
-        <v>279</v>
-      </c>
       <c r="I70" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3637,16 +3637,16 @@
         <v>6</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D71" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E71" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I71" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3657,22 +3657,22 @@
         <v>6</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D72" t="s">
+        <v>280</v>
+      </c>
+      <c r="E72" t="s">
+        <v>281</v>
+      </c>
+      <c r="G72" t="s">
         <v>282</v>
       </c>
-      <c r="D72" t="s">
+      <c r="H72" t="s">
         <v>283</v>
       </c>
-      <c r="E72" t="s">
-        <v>284</v>
-      </c>
-      <c r="G72" t="s">
-        <v>285</v>
-      </c>
-      <c r="H72" t="s">
-        <v>286</v>
-      </c>
       <c r="I72" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3683,22 +3683,22 @@
         <v>2</v>
       </c>
       <c r="C73" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D73" t="s">
+        <v>285</v>
+      </c>
+      <c r="E73" t="s">
+        <v>286</v>
+      </c>
+      <c r="G73" t="s">
         <v>287</v>
       </c>
-      <c r="D73" t="s">
+      <c r="H73" t="s">
         <v>288</v>
       </c>
-      <c r="E73" t="s">
-        <v>289</v>
-      </c>
-      <c r="G73" t="s">
-        <v>290</v>
-      </c>
-      <c r="H73" t="s">
-        <v>291</v>
-      </c>
       <c r="I73" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3709,22 +3709,22 @@
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D74" t="s">
+        <v>290</v>
+      </c>
+      <c r="E74" t="s">
+        <v>291</v>
+      </c>
+      <c r="G74" t="s">
         <v>292</v>
       </c>
-      <c r="D74" t="s">
+      <c r="H74" t="s">
         <v>293</v>
       </c>
-      <c r="E74" t="s">
+      <c r="I74" t="s">
         <v>294</v>
-      </c>
-      <c r="G74" t="s">
-        <v>295</v>
-      </c>
-      <c r="H74" t="s">
-        <v>296</v>
-      </c>
-      <c r="I74" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>